<commit_message>
check metro 52 and output all in QGIS
</commit_message>
<xml_diff>
--- a/data/Metro 52 Zuid = Noord.xlsx
+++ b/data/Metro 52 Zuid = Noord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UTNCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89361A99-9FAD-4349-9B2A-02E09B042C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432C5216-7D32-4AF9-AA3A-C06A8208C4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,54 +25,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>Station Zuid</t>
+  </si>
+  <si>
+    <t>13:31 + 1</t>
+  </si>
+  <si>
+    <t>13:38 + 1</t>
+  </si>
+  <si>
+    <t>Europaplein</t>
+  </si>
+  <si>
+    <t>13:33 + 1</t>
+  </si>
+  <si>
+    <t>13:41 + 1</t>
+  </si>
+  <si>
+    <t>De Pijp</t>
+  </si>
+  <si>
+    <t>13:35 + 1</t>
+  </si>
+  <si>
+    <t>13:43 + 1</t>
+  </si>
+  <si>
+    <t>Vijzelgracht</t>
+  </si>
+  <si>
+    <t>13:37 + 1</t>
+  </si>
+  <si>
+    <t>13:44 + 1</t>
+  </si>
+  <si>
+    <t>Rokin</t>
+  </si>
+  <si>
+    <t>13:39 + 1</t>
+  </si>
+  <si>
+    <t>13:46 + 1</t>
+  </si>
+  <si>
+    <t>Centraal Station</t>
+  </si>
+  <si>
+    <t>Noorderpark</t>
+  </si>
   <si>
     <t>Noord</t>
   </si>
   <si>
-    <t>13:35 + 1</t>
-  </si>
-  <si>
-    <t>13:43 + 1</t>
-  </si>
-  <si>
-    <t>Noorderpark</t>
-  </si>
-  <si>
-    <t>13:37 + 1</t>
-  </si>
-  <si>
     <t>13:45 + 1</t>
-  </si>
-  <si>
-    <t>Centraal Station</t>
-  </si>
-  <si>
-    <t>13:40 + 1</t>
-  </si>
-  <si>
-    <t>13:47 + 1</t>
-  </si>
-  <si>
-    <t>Rokin</t>
-  </si>
-  <si>
-    <t>13:42 + 1</t>
-  </si>
-  <si>
-    <t>Vijzelgracht</t>
-  </si>
-  <si>
-    <t>13:44 + 1</t>
-  </si>
-  <si>
-    <t>De Pijp</t>
-  </si>
-  <si>
-    <t>Europaplein</t>
-  </si>
-  <si>
-    <t>Station Zuid</t>
   </si>
 </sst>
 </file>
@@ -416,7 +425,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.57638888888888895</v>
+        <v>0.57361111111111118</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -436,7 +445,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.57777777777777783</v>
+        <v>0.57500000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -456,7 +465,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0.57986111111111105</v>
+        <v>0.57638888888888895</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -470,38 +479,38 @@
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.5756944444444444</v>
+      <c r="A15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>0.58124999999999993</v>
+        <v>0.57777777777777783</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.57708333333333328</v>
+      <c r="A19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.58263888888888882</v>
+        <v>0.57916666666666672</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -511,17 +520,17 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>0.57847222222222217</v>
+        <v>0.57500000000000007</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.58333333333333337</v>
+        <v>0.5805555555555556</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -531,32 +540,32 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>0.57986111111111105</v>
+        <v>0.57638888888888895</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>0.58472222222222225</v>
+        <v>0.58194444444444449</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0.57638888888888895</v>
+      <c r="A30" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>0.58124999999999993</v>
+        <v>0.57847222222222217</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>0.58680555555555558</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>